<commit_message>
last addition to apis
</commit_message>
<xml_diff>
--- a/xls_grupos/CAF_GrupoAstronomo.xlsx
+++ b/xls_grupos/CAF_GrupoAstronomo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaros/Documents/MATLAB/PersonalProjects/Cosecha_Colectiva/xls_grupos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74D07E3-8918-8445-9E4C-D5063BEC6821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C1A4E4-87BD-9246-A1C7-0CF37A33399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -834,8 +834,8 @@
   </sheetPr>
   <dimension ref="A1:Z970"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4721,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9F43F-D256-544F-9E99-A23C28176CED}">
   <dimension ref="A3:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="17">
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="D54" s="17">
         <v>0</v>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="C61" s="19">
         <f>SUM(C50:C59)</f>
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="D61" s="19">
         <f>SUM(D50:D59)</f>

</xml_diff>

<commit_message>
Almost update to db working
</commit_message>
<xml_diff>
--- a/xls_grupos/CAF_GrupoAstronomo.xlsx
+++ b/xls_grupos/CAF_GrupoAstronomo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaros/Documents/MATLAB/PersonalProjects/Cosecha_Colectiva/xls_grupos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C1A4E4-87BD-9246-A1C7-0CF37A33399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244FC9F1-F114-364D-8E55-0BAB4B0C9727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="107">
   <si>
     <t>Nombres</t>
   </si>
@@ -190,9 +192,6 @@
     <t>Id_socio_administrador_suplente</t>
   </si>
   <si>
-    <t>2022-11-10</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -296,9 +295,6 @@
   </si>
   <si>
     <t>RETIRO_ACCIONES</t>
-  </si>
-  <si>
-    <t>2023-11-10</t>
   </si>
   <si>
     <t>3</t>
@@ -368,6 +364,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -609,6 +608,8 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,13 +919,13 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>23</v>
@@ -972,7 +973,7 @@
         <v>32</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="T2" s="3">
         <v>12345</v>
@@ -986,13 +987,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>23</v>
@@ -1040,7 +1041,7 @@
         <v>32</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T3" s="3">
         <v>12345</v>
@@ -1054,13 +1055,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
@@ -1108,7 +1109,7 @@
         <v>32</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="T4" s="3">
         <v>12345</v>
@@ -1122,13 +1123,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
@@ -1176,7 +1177,7 @@
         <v>32</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="T5" s="3">
         <v>12345</v>
@@ -1190,13 +1191,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
@@ -1244,7 +1245,7 @@
         <v>32</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T6" s="3">
         <v>12345</v>
@@ -1258,13 +1259,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>23</v>
@@ -1312,7 +1313,7 @@
         <v>32</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T7" s="3">
         <v>12345</v>
@@ -1326,13 +1327,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
@@ -1380,7 +1381,7 @@
         <v>32</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T8" s="3">
         <v>12345</v>
@@ -1394,13 +1395,13 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>23</v>
@@ -1448,7 +1449,7 @@
         <v>32</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T9" s="3">
         <v>12345</v>
@@ -1462,13 +1463,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>23</v>
@@ -1516,7 +1517,7 @@
         <v>32</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T10" s="3">
         <v>12345</v>
@@ -1530,13 +1531,13 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>23</v>
@@ -1584,7 +1585,7 @@
         <v>32</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T11" s="3">
         <v>12345</v>
@@ -4505,10 +4506,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E24" sqref="E24:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4589,56 +4590,57 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="49">
+        <f ca="1">DATE(YEAR(TODAY())+1,MONTH(TODAY()),DAY(TODAY()))</f>
+        <v>45550</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -4651,56 +4653,57 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>87</v>
+      <c r="A3" s="49">
+        <f ca="1">DATE(YEAR(TODAY())+1,MONTH(TODAY()),DAY(TODAY()))</f>
+        <v>45550</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -4712,6 +4715,9 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
+    <row r="30" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="48"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4721,8 +4727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9F43F-D256-544F-9E99-A23C28176CED}">
   <dimension ref="A3:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4733,7 +4739,7 @@
     <row r="3" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -4750,46 +4756,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -5257,7 +5263,7 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="15">
         <f t="shared" ref="C16:N16" si="0">SUM(C5:C15)</f>
@@ -5311,7 +5317,7 @@
     <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -5328,46 +5334,46 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="D19" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="E19" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="F19" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="G19" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="H19" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="I19" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="J19" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="K19" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="L19" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="M19" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="M19" s="25" t="s">
+      <c r="N19" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -5811,7 +5817,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="27">
         <f t="shared" ref="C31:N31" si="1">SUM(C20:C29)</f>
@@ -5865,7 +5871,7 @@
     <row r="33" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
@@ -5882,46 +5888,46 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="H34" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="I34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="J34" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="K34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="K34" s="10" t="s">
+      <c r="L34" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="M34" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M34" s="10" t="s">
+      <c r="N34" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="N34" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -6125,7 +6131,7 @@
         <v>50</v>
       </c>
       <c r="L39" s="21">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M39" s="21">
         <v>0</v>
@@ -6365,7 +6371,7 @@
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="23"/>
       <c r="B46" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="23">
         <f t="shared" ref="C46:N46" si="2">SUM(C35:C44)</f>
@@ -6405,7 +6411,7 @@
       </c>
       <c r="L46" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="2"/>
@@ -6419,7 +6425,7 @@
     <row r="48" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -6436,46 +6442,46 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="45" t="s">
+      <c r="D49" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="45" t="s">
+      <c r="E49" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="45" t="s">
+      <c r="F49" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="F49" s="45" t="s">
+      <c r="G49" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="G49" s="45" t="s">
+      <c r="H49" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="H49" s="45" t="s">
+      <c r="I49" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="45" t="s">
+      <c r="J49" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="J49" s="45" t="s">
+      <c r="K49" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="K49" s="45" t="s">
+      <c r="L49" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="L49" s="45" t="s">
+      <c r="M49" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="M49" s="45" t="s">
+      <c r="N49" s="45" t="s">
         <v>72</v>
-      </c>
-      <c r="N49" s="45" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -6652,7 +6658,7 @@
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="17">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D54" s="17">
         <v>0</v>
@@ -6919,11 +6925,11 @@
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
       <c r="B61" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" s="19">
         <f>SUM(C50:C59)</f>
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D61" s="19">
         <f>SUM(D50:D59)</f>
@@ -6973,11 +6979,11 @@
     <row r="63" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A63" s="33"/>
       <c r="B63" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="33"/>
       <c r="D63" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E63" s="33"/>
       <c r="F63" s="33"/>
@@ -6992,46 +6998,46 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="46" t="s">
+      <c r="D64" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D64" s="46" t="s">
+      <c r="E64" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="E64" s="46" t="s">
+      <c r="F64" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="46" t="s">
+      <c r="G64" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="G64" s="46" t="s">
+      <c r="H64" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="H64" s="46" t="s">
+      <c r="I64" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="I64" s="46" t="s">
+      <c r="J64" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J64" s="46" t="s">
+      <c r="K64" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="K64" s="46" t="s">
+      <c r="L64" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L64" s="46" t="s">
+      <c r="M64" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="M64" s="46" t="s">
+      <c r="N64" s="46" t="s">
         <v>72</v>
-      </c>
-      <c r="N64" s="46" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -7475,7 +7481,7 @@
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="38"/>
       <c r="B76" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="38">
         <f>SUM(C65:C74)</f>
@@ -7529,11 +7535,11 @@
     <row r="78" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A78" s="33"/>
       <c r="B78" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C78" s="33"/>
       <c r="D78" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E78" s="33"/>
       <c r="F78" s="33"/>
@@ -7548,46 +7554,46 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B79" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C79" s="46" t="s">
+      <c r="D79" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D79" s="46" t="s">
+      <c r="E79" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="E79" s="46" t="s">
+      <c r="F79" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="F79" s="46" t="s">
+      <c r="G79" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="G79" s="46" t="s">
+      <c r="H79" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="H79" s="46" t="s">
+      <c r="I79" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="I79" s="46" t="s">
+      <c r="J79" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J79" s="46" t="s">
+      <c r="K79" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="K79" s="46" t="s">
+      <c r="L79" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L79" s="46" t="s">
+      <c r="M79" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="M79" s="46" t="s">
+      <c r="N79" s="46" t="s">
         <v>72</v>
-      </c>
-      <c r="N79" s="46" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -8031,7 +8037,7 @@
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="38"/>
       <c r="B91" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C91" s="38">
         <f>SUM(C80:C89)</f>
@@ -8085,7 +8091,7 @@
     <row r="93" spans="1:14" ht="26" x14ac:dyDescent="0.3">
       <c r="A93" s="39"/>
       <c r="B93" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C93" s="39"/>
       <c r="D93" s="39"/>
@@ -8102,46 +8108,46 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B94" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C94" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C94" s="47" t="s">
+      <c r="D94" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="D94" s="47" t="s">
+      <c r="E94" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E94" s="47" t="s">
+      <c r="F94" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="F94" s="47" t="s">
+      <c r="G94" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="G94" s="47" t="s">
+      <c r="H94" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="H94" s="47" t="s">
+      <c r="I94" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="I94" s="47" t="s">
+      <c r="J94" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="J94" s="47" t="s">
+      <c r="K94" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="K94" s="47" t="s">
+      <c r="L94" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="L94" s="47" t="s">
+      <c r="M94" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="M94" s="47" t="s">
+      <c r="N94" s="47" t="s">
         <v>72</v>
-      </c>
-      <c r="N94" s="47" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -8585,7 +8591,7 @@
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="44"/>
       <c r="B106" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C106" s="44">
         <f>SUM(C95:C104)</f>
@@ -8639,7 +8645,7 @@
     <row r="108" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A108" s="24"/>
       <c r="B108" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C108" s="24"/>
       <c r="D108" s="24"/>
@@ -8656,46 +8662,46 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B109" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C109" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C109" s="25" t="s">
+      <c r="D109" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D109" s="25" t="s">
+      <c r="E109" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E109" s="25" t="s">
+      <c r="F109" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F109" s="25" t="s">
+      <c r="G109" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="G109" s="25" t="s">
+      <c r="H109" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H109" s="25" t="s">
+      <c r="I109" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I109" s="25" t="s">
+      <c r="J109" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="J109" s="25" t="s">
+      <c r="K109" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="K109" s="25" t="s">
+      <c r="L109" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="L109" s="25" t="s">
+      <c r="M109" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="M109" s="25" t="s">
+      <c r="N109" s="25" t="s">
         <v>72</v>
-      </c>
-      <c r="N109" s="25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -9139,7 +9145,7 @@
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="27"/>
       <c r="B121" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C121" s="27">
         <f t="shared" ref="C121:N121" si="7">SUM(C110:C119)</f>
@@ -9193,7 +9199,7 @@
     <row r="124" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A124" s="28"/>
       <c r="B124" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -9210,46 +9216,46 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B125" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C125" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C125" s="30" t="s">
+      <c r="D125" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D125" s="30" t="s">
+      <c r="E125" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E125" s="30" t="s">
+      <c r="F125" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F125" s="30" t="s">
+      <c r="G125" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G125" s="30" t="s">
+      <c r="H125" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H125" s="30" t="s">
+      <c r="I125" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="I125" s="30" t="s">
+      <c r="J125" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="J125" s="30" t="s">
+      <c r="K125" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="K125" s="30" t="s">
+      <c r="L125" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="L125" s="30" t="s">
+      <c r="M125" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="M125" s="30" t="s">
+      <c r="N125" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="N125" s="30" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
@@ -9297,7 +9303,7 @@
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="32"/>
       <c r="B127" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C127" s="32">
         <f t="shared" ref="C127:N127" si="8">SUM(C126:C126)</f>

</xml_diff>